<commit_message>
returning header and data errors to component
</commit_message>
<xml_diff>
--- a/pakker-v2.xlsx
+++ b/pakker-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heeids\Documents\Ciber-prosjekter\ETA-Posten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52BFE3A-A73B-48A7-BEB8-511A7E286FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6854CB-8C70-4409-99BD-711CA7093EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11235" yWindow="9315" windowWidth="17670" windowHeight="9975" xr2:uid="{003C0448-2027-4768-852F-48A222163C0B}"/>
+    <workbookView xWindow="14340" yWindow="6750" windowWidth="17670" windowHeight="9975" xr2:uid="{003C0448-2027-4768-852F-48A222163C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="94">
   <si>
     <t/>
   </si>
@@ -700,7 +700,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,8 +1023,8 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>123</v>
+      <c r="A6" t="s">
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
checks if postal code is valid postal code
</commit_message>
<xml_diff>
--- a/pakker-v2.xlsx
+++ b/pakker-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heeids\Documents\Ciber-prosjekter\ETA-Posten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA2A6D9-1F47-4565-B92F-5D7BF43614CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820CD326-18BA-47E7-8BA7-F4ACBD1A021E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16725" yWindow="10875" windowWidth="17655" windowHeight="9975" xr2:uid="{003C0448-2027-4768-852F-48A222163C0B}"/>
+    <workbookView xWindow="8775" yWindow="7995" windowWidth="20220" windowHeight="11520" xr2:uid="{003C0448-2027-4768-852F-48A222163C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -9013,7 +9013,7 @@
   <dimension ref="A1:Q1130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed validation for new column referencing
</commit_message>
<xml_diff>
--- a/pakker-v2.xlsx
+++ b/pakker-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heeids\Documents\Ciber-prosjekter\ETA-Posten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820CD326-18BA-47E7-8BA7-F4ACBD1A021E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED99F87-B931-4A4A-B0B9-B89C7E845BDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8775" yWindow="7995" windowWidth="20220" windowHeight="11520" xr2:uid="{003C0448-2027-4768-852F-48A222163C0B}"/>
+    <workbookView xWindow="3375" yWindow="4515" windowWidth="20220" windowHeight="11520" xr2:uid="{003C0448-2027-4768-852F-48A222163C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -9013,7 +9013,7 @@
   <dimension ref="A1:Q1130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>